<commit_message>
new china figures on pop by age
</commit_message>
<xml_diff>
--- a/china/data/raw/un_china_age_cohort_projections.xlsx
+++ b/china/data/raw/un_china_age_cohort_projections.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stiles/github/notebooks/china/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF986FC6-B75F-1149-979B-77B48B03E912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4471D02A-CCCE-1F49-9AB6-747079608604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{E5332244-D14D-E043-90EF-37366BFA949B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38000" windowHeight="21020" activeTab="1" xr2:uid="{E5332244-D14D-E043-90EF-37366BFA949B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="16">
   <si>
     <t>&lt; 15</t>
   </si>
@@ -51,12 +52,48 @@
   <si>
     <t>Year</t>
   </si>
+  <si>
+    <t>Reference date (as of 1 July)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>0-14</t>
+  </si>
+  <si>
+    <t>15+</t>
+  </si>
+  <si>
+    <t>15-64</t>
+  </si>
+  <si>
+    <t>65+</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>0-15</t>
+  </si>
+  <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#\ ###\ ###\ ##0;\-#\ ###\ ###\ ##0;0"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -64,19 +101,97 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -85,8 +200,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC422390-32BA-2843-884C-75A120386A58}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -638,12 +792,1627 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE0C3E7C-D14C-C747-B6B4-609C61E93AA5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="A1:H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="62.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="62.6640625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="13">
+        <v>1950</v>
+      </c>
+      <c r="C2" s="6">
+        <v>55441926.899999999</v>
+      </c>
+      <c r="D2" s="6">
+        <v>18873029.5</v>
+      </c>
+      <c r="E2" s="6">
+        <v>36568897.399999999</v>
+      </c>
+      <c r="F2" s="6">
+        <v>34113148.200000003</v>
+      </c>
+      <c r="G2" s="6">
+        <v>24262679.5</v>
+      </c>
+      <c r="H2" s="6">
+        <v>2455749.1999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1955</v>
+      </c>
+      <c r="C3" s="6">
+        <v>61224155.200000003</v>
+      </c>
+      <c r="D3" s="6">
+        <v>23030644.099999998</v>
+      </c>
+      <c r="E3" s="6">
+        <v>38193511.099999994</v>
+      </c>
+      <c r="F3" s="6">
+        <v>35713389.600000001</v>
+      </c>
+      <c r="G3" s="6">
+        <v>25302691.899999999</v>
+      </c>
+      <c r="H3" s="6">
+        <v>2480121.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1960</v>
+      </c>
+      <c r="C4" s="6">
+        <v>66040805.399999999</v>
+      </c>
+      <c r="D4" s="6">
+        <v>26298896.299999997</v>
+      </c>
+      <c r="E4" s="6">
+        <v>39741909.100000001</v>
+      </c>
+      <c r="F4" s="6">
+        <v>37305987.5</v>
+      </c>
+      <c r="G4" s="6">
+        <v>26694747.100000001</v>
+      </c>
+      <c r="H4" s="6">
+        <v>2435921.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1965</v>
+      </c>
+      <c r="C5" s="6">
+        <v>72421897</v>
+      </c>
+      <c r="D5" s="6">
+        <v>29822204.399999999</v>
+      </c>
+      <c r="E5" s="6">
+        <v>42599692.599999994</v>
+      </c>
+      <c r="F5" s="6">
+        <v>40120143.800000004</v>
+      </c>
+      <c r="G5" s="6">
+        <v>28153689.600000001</v>
+      </c>
+      <c r="H5" s="6">
+        <v>2479548.8000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1970</v>
+      </c>
+      <c r="C6" s="6">
+        <v>82760138.5</v>
+      </c>
+      <c r="D6" s="6">
+        <v>33441072.899999999</v>
+      </c>
+      <c r="E6" s="6">
+        <v>49319065.600000001</v>
+      </c>
+      <c r="F6" s="6">
+        <v>46217193.5</v>
+      </c>
+      <c r="G6" s="6">
+        <v>30279206.400000002</v>
+      </c>
+      <c r="H6" s="6">
+        <v>3101872.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1975</v>
+      </c>
+      <c r="C7" s="6">
+        <v>92624088.899999991</v>
+      </c>
+      <c r="D7" s="6">
+        <v>36902647.700000003</v>
+      </c>
+      <c r="E7" s="6">
+        <v>55721441.200000003</v>
+      </c>
+      <c r="F7" s="6">
+        <v>51938254.5</v>
+      </c>
+      <c r="G7" s="6">
+        <v>33815733.600000001</v>
+      </c>
+      <c r="H7" s="6">
+        <v>3783186.6999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1980</v>
+      </c>
+      <c r="C8" s="6">
+        <v>100008922.8</v>
+      </c>
+      <c r="D8" s="6">
+        <v>35938726.799999997</v>
+      </c>
+      <c r="E8" s="6">
+        <v>64070196</v>
+      </c>
+      <c r="F8" s="6">
+        <v>59395446.100000001</v>
+      </c>
+      <c r="G8" s="6">
+        <v>39772678.399999999</v>
+      </c>
+      <c r="H8" s="6">
+        <v>4674749.9000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1985</v>
+      </c>
+      <c r="C9" s="6">
+        <v>107558936.29999998</v>
+      </c>
+      <c r="D9" s="6">
+        <v>33059569.600000001</v>
+      </c>
+      <c r="E9" s="6">
+        <v>74499366.700000003</v>
+      </c>
+      <c r="F9" s="6">
+        <v>68788053.400000006</v>
+      </c>
+      <c r="G9" s="6">
+        <v>44953772.200000003</v>
+      </c>
+      <c r="H9" s="6">
+        <v>5711313.2999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1990</v>
+      </c>
+      <c r="C10" s="6">
+        <v>117688368.10000001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>33646770.899999999</v>
+      </c>
+      <c r="E10" s="6">
+        <v>84041597.199999988</v>
+      </c>
+      <c r="F10" s="6">
+        <v>77415550.799999997</v>
+      </c>
+      <c r="G10" s="6">
+        <v>51860633.700000003</v>
+      </c>
+      <c r="H10" s="6">
+        <v>6626046.4000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1995</v>
+      </c>
+      <c r="C11" s="6">
+        <v>124092053.90000001</v>
+      </c>
+      <c r="D11" s="6">
+        <v>33544769.400000002</v>
+      </c>
+      <c r="E11" s="6">
+        <v>90547284.5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>82947509.099999994</v>
+      </c>
+      <c r="G11" s="6">
+        <v>60536724.199999996</v>
+      </c>
+      <c r="H11" s="6">
+        <v>7599775.4000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13">
+        <v>2000</v>
+      </c>
+      <c r="C12" s="6">
+        <v>129055076.7</v>
+      </c>
+      <c r="D12" s="6">
+        <v>31991102.800000001</v>
+      </c>
+      <c r="E12" s="6">
+        <v>97063973.899999991</v>
+      </c>
+      <c r="F12" s="6">
+        <v>88272932.200000003</v>
+      </c>
+      <c r="G12" s="6">
+        <v>68077470.599999994</v>
+      </c>
+      <c r="H12" s="6">
+        <v>8791041.6999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13">
+        <v>2005</v>
+      </c>
+      <c r="C13" s="6">
+        <v>133077637.99999999</v>
+      </c>
+      <c r="D13" s="6">
+        <v>27085889.899999999</v>
+      </c>
+      <c r="E13" s="6">
+        <v>105991748.09999999</v>
+      </c>
+      <c r="F13" s="6">
+        <v>96034252.5</v>
+      </c>
+      <c r="G13" s="6">
+        <v>72731639.099999994</v>
+      </c>
+      <c r="H13" s="6">
+        <v>9957495.6000000015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="13">
+        <v>2010</v>
+      </c>
+      <c r="C14" s="6">
+        <v>136881060.40000001</v>
+      </c>
+      <c r="D14" s="6">
+        <v>25541947.399999999</v>
+      </c>
+      <c r="E14" s="6">
+        <v>111339112.99999999</v>
+      </c>
+      <c r="F14" s="6">
+        <v>100286716.5</v>
+      </c>
+      <c r="G14" s="6">
+        <v>77360752.200000003</v>
+      </c>
+      <c r="H14" s="6">
+        <v>11052396.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="13">
+        <v>2015</v>
+      </c>
+      <c r="C15" s="6">
+        <v>140684786.80000001</v>
+      </c>
+      <c r="D15" s="6">
+        <v>25399000.899999999</v>
+      </c>
+      <c r="E15" s="6">
+        <v>115285785.89999999</v>
+      </c>
+      <c r="F15" s="6">
+        <v>102157320.40000001</v>
+      </c>
+      <c r="G15" s="6">
+        <v>83530335.700000003</v>
+      </c>
+      <c r="H15" s="6">
+        <v>13128465.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="13">
+        <v>2020</v>
+      </c>
+      <c r="C16" s="6">
+        <v>143932377.40000001</v>
+      </c>
+      <c r="D16" s="6">
+        <v>25493037.100000001</v>
+      </c>
+      <c r="E16" s="6">
+        <v>118439340.3</v>
+      </c>
+      <c r="F16" s="6">
+        <v>101213122.90000001</v>
+      </c>
+      <c r="G16" s="6">
+        <v>84263120.299999997</v>
+      </c>
+      <c r="H16" s="6">
+        <v>17226217.399999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="13">
+        <v>2020</v>
+      </c>
+      <c r="C17" s="6">
+        <v>143932377.40000001</v>
+      </c>
+      <c r="D17" s="6">
+        <v>25493037.100000001</v>
+      </c>
+      <c r="E17" s="6">
+        <v>118439340.3</v>
+      </c>
+      <c r="F17" s="6">
+        <v>101213122.90000001</v>
+      </c>
+      <c r="G17" s="6">
+        <v>84263120.299999997</v>
+      </c>
+      <c r="H17" s="6">
+        <v>17226217.399999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="13">
+        <v>2025</v>
+      </c>
+      <c r="C18" s="6">
+        <v>145790824.79999998</v>
+      </c>
+      <c r="D18" s="6">
+        <v>24668784.800000001</v>
+      </c>
+      <c r="E18" s="6">
+        <v>121122039.99999999</v>
+      </c>
+      <c r="F18" s="6">
+        <v>100664972</v>
+      </c>
+      <c r="G18" s="6">
+        <v>84085882.200000003</v>
+      </c>
+      <c r="H18" s="6">
+        <v>20457068</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="13">
+        <v>2030</v>
+      </c>
+      <c r="C19" s="6">
+        <v>146434015</v>
+      </c>
+      <c r="D19" s="6">
+        <v>23085432</v>
+      </c>
+      <c r="E19" s="6">
+        <v>123348583</v>
+      </c>
+      <c r="F19" s="6">
+        <v>98649977</v>
+      </c>
+      <c r="G19" s="6">
+        <v>81670933</v>
+      </c>
+      <c r="H19" s="6">
+        <v>24698606</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="13">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="6">
+        <v>146108303</v>
+      </c>
+      <c r="D20" s="6">
+        <v>21565860</v>
+      </c>
+      <c r="E20" s="6">
+        <v>124542443</v>
+      </c>
+      <c r="F20" s="6">
+        <v>94332961.700000003</v>
+      </c>
+      <c r="G20" s="6">
+        <v>77407161.100000009</v>
+      </c>
+      <c r="H20" s="6">
+        <v>30209481.300000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="13">
+        <v>2040</v>
+      </c>
+      <c r="C21" s="6">
+        <v>144903142</v>
+      </c>
+      <c r="D21" s="6">
+        <v>20684084.599999998</v>
+      </c>
+      <c r="E21" s="6">
+        <v>124219057.40000001</v>
+      </c>
+      <c r="F21" s="6">
+        <v>89837145.599999994</v>
+      </c>
+      <c r="G21" s="6">
+        <v>73955020.799999997</v>
+      </c>
+      <c r="H21" s="6">
+        <v>34381911.800000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="13">
+        <v>2045</v>
+      </c>
+      <c r="C22" s="6">
+        <v>142931224.5</v>
+      </c>
+      <c r="D22" s="6">
+        <v>20241555.900000002</v>
+      </c>
+      <c r="E22" s="6">
+        <v>122689668.59999999</v>
+      </c>
+      <c r="F22" s="6">
+        <v>87103262.5</v>
+      </c>
+      <c r="G22" s="6">
+        <v>72497469.599999994</v>
+      </c>
+      <c r="H22" s="6">
+        <v>35586406.100000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="13">
+        <v>2050</v>
+      </c>
+      <c r="C23" s="6">
+        <v>140240516.69999999</v>
+      </c>
+      <c r="D23" s="6">
+        <v>19838993.699999999</v>
+      </c>
+      <c r="E23" s="6">
+        <v>120401523</v>
+      </c>
+      <c r="F23" s="6">
+        <v>83837901.399999991</v>
+      </c>
+      <c r="G23" s="6">
+        <v>69990851</v>
+      </c>
+      <c r="H23" s="6">
+        <v>36563621.600000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="13">
+        <v>2055</v>
+      </c>
+      <c r="C24" s="6">
+        <v>136959414.29999998</v>
+      </c>
+      <c r="D24" s="6">
+        <v>19319898</v>
+      </c>
+      <c r="E24" s="6">
+        <v>117639516.3</v>
+      </c>
+      <c r="F24" s="6">
+        <v>77925212.100000009</v>
+      </c>
+      <c r="G24" s="6">
+        <v>64428003.099999994</v>
+      </c>
+      <c r="H24" s="6">
+        <v>39714304.200000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="13">
+        <v>2060</v>
+      </c>
+      <c r="C25" s="6">
+        <v>133303063.2</v>
+      </c>
+      <c r="D25" s="6">
+        <v>18658725.399999999</v>
+      </c>
+      <c r="E25" s="6">
+        <v>114644337.8</v>
+      </c>
+      <c r="F25" s="6">
+        <v>74875558.900000006</v>
+      </c>
+      <c r="G25" s="6">
+        <v>61582172.299999997</v>
+      </c>
+      <c r="H25" s="6">
+        <v>39768778.899999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="13">
+        <v>2065</v>
+      </c>
+      <c r="C26" s="6">
+        <v>129528457.5</v>
+      </c>
+      <c r="D26" s="6">
+        <v>17998508.600000001</v>
+      </c>
+      <c r="E26" s="6">
+        <v>111529948.90000001</v>
+      </c>
+      <c r="F26" s="6">
+        <v>72699025.399999991</v>
+      </c>
+      <c r="G26" s="6">
+        <v>59687873</v>
+      </c>
+      <c r="H26" s="6">
+        <v>38830923.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="13">
+        <v>2070</v>
+      </c>
+      <c r="C27" s="6">
+        <v>125805422.3</v>
+      </c>
+      <c r="D27" s="6">
+        <v>17425399.400000002</v>
+      </c>
+      <c r="E27" s="6">
+        <v>108380022.90000001</v>
+      </c>
+      <c r="F27" s="6">
+        <v>70776693.099999994</v>
+      </c>
+      <c r="G27" s="6">
+        <v>58193321</v>
+      </c>
+      <c r="H27" s="6">
+        <v>37603329.800000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="13">
+        <v>2075</v>
+      </c>
+      <c r="C28" s="6">
+        <v>122158015.3</v>
+      </c>
+      <c r="D28" s="6">
+        <v>16948667</v>
+      </c>
+      <c r="E28" s="6">
+        <v>105209348.3</v>
+      </c>
+      <c r="F28" s="6">
+        <v>68460678.5</v>
+      </c>
+      <c r="G28" s="6">
+        <v>56340630.500000007</v>
+      </c>
+      <c r="H28" s="6">
+        <v>36748669.799999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="13">
+        <v>2080</v>
+      </c>
+      <c r="C29" s="6">
+        <v>118589129.7</v>
+      </c>
+      <c r="D29" s="6">
+        <v>16529714.1</v>
+      </c>
+      <c r="E29" s="6">
+        <v>102059415.59999999</v>
+      </c>
+      <c r="F29" s="6">
+        <v>65726868.000000007</v>
+      </c>
+      <c r="G29" s="6">
+        <v>54031038.800000004</v>
+      </c>
+      <c r="H29" s="6">
+        <v>36332547.600000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="13">
+        <v>2085</v>
+      </c>
+      <c r="C30" s="6">
+        <v>115179920.39999999</v>
+      </c>
+      <c r="D30" s="6">
+        <v>16097940.700000001</v>
+      </c>
+      <c r="E30" s="6">
+        <v>99081979.700000003</v>
+      </c>
+      <c r="F30" s="6">
+        <v>63130747.100000001</v>
+      </c>
+      <c r="G30" s="6">
+        <v>51775569.900000006</v>
+      </c>
+      <c r="H30" s="6">
+        <v>35951232.600000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="13">
+        <v>2090</v>
+      </c>
+      <c r="C31" s="6">
+        <v>112046692.80000001</v>
+      </c>
+      <c r="D31" s="6">
+        <v>15631208.600000001</v>
+      </c>
+      <c r="E31" s="6">
+        <v>96415484.199999988</v>
+      </c>
+      <c r="F31" s="6">
+        <v>61120960</v>
+      </c>
+      <c r="G31" s="6">
+        <v>50046512.399999999</v>
+      </c>
+      <c r="H31" s="6">
+        <v>35294524.200000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="13">
+        <v>2095</v>
+      </c>
+      <c r="C32" s="6">
+        <v>109211520.09999999</v>
+      </c>
+      <c r="D32" s="6">
+        <v>15144510.999999998</v>
+      </c>
+      <c r="E32" s="6">
+        <v>94067009.099999994</v>
+      </c>
+      <c r="F32" s="6">
+        <v>59478466.700000003</v>
+      </c>
+      <c r="G32" s="6">
+        <v>48674660.899999999</v>
+      </c>
+      <c r="H32" s="6">
+        <v>34588542.399999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="13">
+        <v>2100</v>
+      </c>
+      <c r="C33" s="6">
+        <v>106499345.69999999</v>
+      </c>
+      <c r="D33" s="6">
+        <v>14681306.099999998</v>
+      </c>
+      <c r="E33" s="6">
+        <v>91818039.599999994</v>
+      </c>
+      <c r="F33" s="6">
+        <v>57901236.699999996</v>
+      </c>
+      <c r="G33" s="6">
+        <v>47393517.700000003</v>
+      </c>
+      <c r="H33" s="6">
+        <v>33916802.899999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B33">
+    <sortCondition ref="B2:B33"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3283EEDE-989D-B840-BF5C-BD00EF936077}">
+  <dimension ref="A1:R19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:18" ht="39" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1950</v>
+      </c>
+      <c r="B2" s="7">
+        <v>554419.26899999997</v>
+      </c>
+      <c r="C2" s="4">
+        <v>188730.29500000001</v>
+      </c>
+      <c r="D2" s="7">
+        <v>365688.97399999999</v>
+      </c>
+      <c r="E2" s="7">
+        <v>341131.48200000002</v>
+      </c>
+      <c r="F2" s="7">
+        <v>242626.79500000001</v>
+      </c>
+      <c r="G2" s="7">
+        <v>24557.491999999998</v>
+      </c>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>1955</v>
+      </c>
+      <c r="B3" s="7">
+        <v>612241.55200000003</v>
+      </c>
+      <c r="C3" s="4">
+        <v>230306.44099999999</v>
+      </c>
+      <c r="D3" s="7">
+        <v>381935.11099999998</v>
+      </c>
+      <c r="E3" s="7">
+        <v>357133.89600000001</v>
+      </c>
+      <c r="F3" s="7">
+        <v>253026.91899999999</v>
+      </c>
+      <c r="G3" s="7">
+        <v>24801.215</v>
+      </c>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>1960</v>
+      </c>
+      <c r="B4" s="7">
+        <v>660408.054</v>
+      </c>
+      <c r="C4" s="4">
+        <v>262988.96299999999</v>
+      </c>
+      <c r="D4" s="7">
+        <v>397419.09100000001</v>
+      </c>
+      <c r="E4" s="7">
+        <v>373059.875</v>
+      </c>
+      <c r="F4" s="7">
+        <v>266947.47100000002</v>
+      </c>
+      <c r="G4" s="7">
+        <v>24359.216</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1965</v>
+      </c>
+      <c r="B5" s="7">
+        <v>724218.97</v>
+      </c>
+      <c r="C5" s="4">
+        <v>298222.04399999999</v>
+      </c>
+      <c r="D5" s="7">
+        <v>425996.92599999998</v>
+      </c>
+      <c r="E5" s="7">
+        <v>401201.43800000002</v>
+      </c>
+      <c r="F5" s="7">
+        <v>281536.89600000001</v>
+      </c>
+      <c r="G5" s="7">
+        <v>24795.488000000001</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="L5">
+        <v>1950</v>
+      </c>
+      <c r="M5">
+        <v>554419.26899999997</v>
+      </c>
+      <c r="N5">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O5">
+        <v>365688.97399999999</v>
+      </c>
+      <c r="P5">
+        <v>341131.48200000002</v>
+      </c>
+      <c r="Q5">
+        <v>242626.79500000001</v>
+      </c>
+      <c r="R5">
+        <v>24557.491999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>1970</v>
+      </c>
+      <c r="B6" s="7">
+        <v>827601.38500000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>334410.72899999999</v>
+      </c>
+      <c r="D6" s="7">
+        <v>493190.65600000002</v>
+      </c>
+      <c r="E6" s="7">
+        <v>462171.935</v>
+      </c>
+      <c r="F6" s="7">
+        <v>302792.06400000001</v>
+      </c>
+      <c r="G6" s="7">
+        <v>31018.721000000001</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="L6">
+        <v>1955</v>
+      </c>
+      <c r="M6">
+        <v>612241.55200000003</v>
+      </c>
+      <c r="N6">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O6">
+        <v>381935.11099999998</v>
+      </c>
+      <c r="P6">
+        <v>357133.89600000001</v>
+      </c>
+      <c r="Q6">
+        <v>253026.91899999999</v>
+      </c>
+      <c r="R6">
+        <v>24801.215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>1975</v>
+      </c>
+      <c r="B7" s="7">
+        <v>926240.88899999997</v>
+      </c>
+      <c r="C7" s="4">
+        <v>369026.47700000001</v>
+      </c>
+      <c r="D7" s="7">
+        <v>557214.41200000001</v>
+      </c>
+      <c r="E7" s="7">
+        <v>519382.54499999998</v>
+      </c>
+      <c r="F7" s="7">
+        <v>338157.33600000001</v>
+      </c>
+      <c r="G7" s="7">
+        <v>37831.866999999998</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="L7">
+        <v>1960</v>
+      </c>
+      <c r="M7">
+        <v>660408.054</v>
+      </c>
+      <c r="N7">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O7">
+        <v>397419.09100000001</v>
+      </c>
+      <c r="P7">
+        <v>373059.875</v>
+      </c>
+      <c r="Q7">
+        <v>266947.47100000002</v>
+      </c>
+      <c r="R7">
+        <v>24359.216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>1980</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1000089.228</v>
+      </c>
+      <c r="C8" s="4">
+        <v>359387.26799999998</v>
+      </c>
+      <c r="D8" s="7">
+        <v>640701.96</v>
+      </c>
+      <c r="E8" s="7">
+        <v>593954.46100000001</v>
+      </c>
+      <c r="F8" s="7">
+        <v>397726.78399999999</v>
+      </c>
+      <c r="G8" s="7">
+        <v>46747.499000000003</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="L8">
+        <v>1965</v>
+      </c>
+      <c r="M8">
+        <v>724218.97</v>
+      </c>
+      <c r="N8">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O8">
+        <v>425996.92599999998</v>
+      </c>
+      <c r="P8">
+        <v>401201.43800000002</v>
+      </c>
+      <c r="Q8">
+        <v>281536.89600000001</v>
+      </c>
+      <c r="R8">
+        <v>24795.488000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>1985</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1075589.3629999999</v>
+      </c>
+      <c r="C9" s="4">
+        <v>330595.696</v>
+      </c>
+      <c r="D9" s="7">
+        <v>744993.66700000002</v>
+      </c>
+      <c r="E9" s="7">
+        <v>687880.53399999999</v>
+      </c>
+      <c r="F9" s="7">
+        <v>449537.72200000001</v>
+      </c>
+      <c r="G9" s="7">
+        <v>57113.133000000002</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="L9">
+        <v>1970</v>
+      </c>
+      <c r="M9">
+        <v>827601.38500000001</v>
+      </c>
+      <c r="N9">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O9">
+        <v>493190.65600000002</v>
+      </c>
+      <c r="P9">
+        <v>462171.935</v>
+      </c>
+      <c r="Q9">
+        <v>302792.06400000001</v>
+      </c>
+      <c r="R9">
+        <v>31018.721000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>1990</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1176883.6810000001</v>
+      </c>
+      <c r="C10" s="4">
+        <v>336467.70899999997</v>
+      </c>
+      <c r="D10" s="7">
+        <v>840415.97199999995</v>
+      </c>
+      <c r="E10" s="7">
+        <v>774155.50800000003</v>
+      </c>
+      <c r="F10" s="7">
+        <v>518606.337</v>
+      </c>
+      <c r="G10" s="7">
+        <v>66260.464000000007</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="L10">
+        <v>1975</v>
+      </c>
+      <c r="M10">
+        <v>926240.88899999997</v>
+      </c>
+      <c r="N10">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O10">
+        <v>557214.41200000001</v>
+      </c>
+      <c r="P10">
+        <v>519382.54499999998</v>
+      </c>
+      <c r="Q10">
+        <v>338157.33600000001</v>
+      </c>
+      <c r="R10">
+        <v>37831.866999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>1995</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1240920.5390000001</v>
+      </c>
+      <c r="C11" s="4">
+        <v>335447.69400000002</v>
+      </c>
+      <c r="D11" s="7">
+        <v>905472.84499999997</v>
+      </c>
+      <c r="E11" s="7">
+        <v>829475.09100000001</v>
+      </c>
+      <c r="F11" s="7">
+        <v>605367.24199999997</v>
+      </c>
+      <c r="G11" s="7">
+        <v>75997.754000000001</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="L11">
+        <v>1980</v>
+      </c>
+      <c r="M11">
+        <v>1000089.228</v>
+      </c>
+      <c r="N11">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O11">
+        <v>640701.96</v>
+      </c>
+      <c r="P11">
+        <v>593954.46100000001</v>
+      </c>
+      <c r="Q11">
+        <v>397726.78399999999</v>
+      </c>
+      <c r="R11">
+        <v>46747.499000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1290550.767</v>
+      </c>
+      <c r="C12" s="4">
+        <v>319911.02799999999</v>
+      </c>
+      <c r="D12" s="7">
+        <v>970639.73899999994</v>
+      </c>
+      <c r="E12" s="7">
+        <v>882729.32200000004</v>
+      </c>
+      <c r="F12" s="7">
+        <v>680774.70600000001</v>
+      </c>
+      <c r="G12" s="7">
+        <v>87910.417000000001</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="L12">
+        <v>1985</v>
+      </c>
+      <c r="M12">
+        <v>1075589.3629999999</v>
+      </c>
+      <c r="N12">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O12">
+        <v>744993.66700000002</v>
+      </c>
+      <c r="P12">
+        <v>687880.53399999999</v>
+      </c>
+      <c r="Q12">
+        <v>449537.72200000001</v>
+      </c>
+      <c r="R12">
+        <v>57113.133000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>2005</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1330776.3799999999</v>
+      </c>
+      <c r="C13" s="4">
+        <v>270858.89899999998</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1059917.4809999999</v>
+      </c>
+      <c r="E13" s="7">
+        <v>960342.52500000002</v>
+      </c>
+      <c r="F13" s="7">
+        <v>727316.39099999995</v>
+      </c>
+      <c r="G13" s="7">
+        <v>99574.956000000006</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="L13">
+        <v>1990</v>
+      </c>
+      <c r="M13">
+        <v>1176883.6810000001</v>
+      </c>
+      <c r="N13">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O13">
+        <v>840415.97199999995</v>
+      </c>
+      <c r="P13">
+        <v>774155.50800000003</v>
+      </c>
+      <c r="Q13">
+        <v>518606.337</v>
+      </c>
+      <c r="R13">
+        <v>66260.464000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>2010</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1368810.6040000001</v>
+      </c>
+      <c r="C14" s="4">
+        <v>255419.47399999999</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1113391.1299999999</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1002867.165</v>
+      </c>
+      <c r="F14" s="7">
+        <v>773607.522</v>
+      </c>
+      <c r="G14" s="7">
+        <v>110523.965</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="L14">
+        <v>1995</v>
+      </c>
+      <c r="M14">
+        <v>1240920.5390000001</v>
+      </c>
+      <c r="N14">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O14">
+        <v>905472.84499999997</v>
+      </c>
+      <c r="P14">
+        <v>829475.09100000001</v>
+      </c>
+      <c r="Q14">
+        <v>605367.24199999997</v>
+      </c>
+      <c r="R14">
+        <v>75997.754000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1406847.868</v>
+      </c>
+      <c r="C15" s="4">
+        <v>253990.00899999999</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1152857.8589999999</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1021573.204</v>
+      </c>
+      <c r="F15" s="7">
+        <v>835303.35699999996</v>
+      </c>
+      <c r="G15" s="7">
+        <v>131284.655</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="L15">
+        <v>2000</v>
+      </c>
+      <c r="M15">
+        <v>1290550.767</v>
+      </c>
+      <c r="N15">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O15">
+        <v>970639.73899999994</v>
+      </c>
+      <c r="P15">
+        <v>882729.32200000004</v>
+      </c>
+      <c r="Q15">
+        <v>680774.70600000001</v>
+      </c>
+      <c r="R15">
+        <v>87910.417000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1439323.774</v>
+      </c>
+      <c r="C16" s="4">
+        <v>254930.37100000001</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1184393.4029999999</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1012131.2290000001</v>
+      </c>
+      <c r="F16" s="7">
+        <v>842631.20299999998</v>
+      </c>
+      <c r="G16" s="7">
+        <v>172262.174</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="L16">
+        <v>2005</v>
+      </c>
+      <c r="M16">
+        <v>1330776.3799999999</v>
+      </c>
+      <c r="N16">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O16">
+        <v>1059917.4809999999</v>
+      </c>
+      <c r="P16">
+        <v>960342.52500000002</v>
+      </c>
+      <c r="Q16">
+        <v>727316.39099999995</v>
+      </c>
+      <c r="R16">
+        <v>99574.956000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>2010</v>
+      </c>
+      <c r="M17">
+        <v>1368810.6040000001</v>
+      </c>
+      <c r="N17">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O17">
+        <v>1113391.1299999999</v>
+      </c>
+      <c r="P17">
+        <v>1002867.165</v>
+      </c>
+      <c r="Q17">
+        <v>773607.522</v>
+      </c>
+      <c r="R17">
+        <v>110523.965</v>
+      </c>
+    </row>
+    <row r="18" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>2015</v>
+      </c>
+      <c r="M18">
+        <v>1406847.868</v>
+      </c>
+      <c r="N18">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O18">
+        <v>1152857.8589999999</v>
+      </c>
+      <c r="P18">
+        <v>1021573.204</v>
+      </c>
+      <c r="Q18">
+        <v>835303.35699999996</v>
+      </c>
+      <c r="R18">
+        <v>131284.655</v>
+      </c>
+    </row>
+    <row r="19" spans="12:18" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <v>2020</v>
+      </c>
+      <c r="M19">
+        <v>1439323.774</v>
+      </c>
+      <c r="N19">
+        <v>188730.29499999998</v>
+      </c>
+      <c r="O19">
+        <v>1184393.4029999999</v>
+      </c>
+      <c r="P19">
+        <v>1012131.2290000001</v>
+      </c>
+      <c r="Q19">
+        <v>842631.20299999998</v>
+      </c>
+      <c r="R19">
+        <v>172262.174</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>